<commit_message>
Revert "Merge pull request #2 from NguyenCongVN/main"
This reverts commit 598d6868ea3174e567ba5a2a081c5b07a4b4c94e, reversing
changes made to 231ca21e70b924096f32f44eaa623d9cf90b6b43.
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QuanLyKhachSan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\QuanLyKhachSanNew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74EA752-B0B0-4144-90D4-49D1CAD7F760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8034211-37C2-4C8E-B8E3-93136C6BDEC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Phân công công việc - Phần mềm quản lý khách sạn</t>
   </si>
@@ -66,40 +66,19 @@
     <t>Xây dựng README.md, LICENSE</t>
   </si>
   <si>
+    <t>Vân</t>
+  </si>
+  <si>
+    <t>Ngọc Tiến</t>
+  </si>
+  <si>
     <t>Công</t>
   </si>
   <si>
-    <t>N Tiến</t>
+    <t>Duy</t>
   </si>
   <si>
     <t>X Tiến</t>
-  </si>
-  <si>
-    <t>Duy</t>
-  </si>
-  <si>
-    <t>Vân</t>
-  </si>
-  <si>
-    <t>21-22/10/2020</t>
-  </si>
-  <si>
-    <t>23-24/10/2020</t>
-  </si>
-  <si>
-    <t>23-26/10/2020</t>
-  </si>
-  <si>
-    <t>27-1/11/2020</t>
-  </si>
-  <si>
-    <t>03-07/11/2020</t>
-  </si>
-  <si>
-    <t>08-015/11/2020</t>
-  </si>
-  <si>
-    <t>16-17/11/2020</t>
   </si>
 </sst>
 </file>
@@ -171,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -181,6 +160,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -190,29 +174,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,7 +466,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,130 +486,114 @@
       <c r="D1" s="3"/>
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" ht="36" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>19</v>
-      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
+      <c r="A7" s="10">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>20</v>
-      </c>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>21</v>
-      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="9">
         <v>6</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+      <c r="A10" s="9">
         <v>7</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="7">
+      <c r="A11" s="10">
         <v>8</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge pull request #2 from NguyenCongVN/main""
This reverts commit ce96e26f00037f98e146996ae3a1cca6d5e3593b.
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\QuanLyKhachSanNew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QuanLyKhachSan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8034211-37C2-4C8E-B8E3-93136C6BDEC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74EA752-B0B0-4144-90D4-49D1CAD7F760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Phân công công việc - Phần mềm quản lý khách sạn</t>
   </si>
@@ -66,19 +66,40 @@
     <t>Xây dựng README.md, LICENSE</t>
   </si>
   <si>
+    <t>Công</t>
+  </si>
+  <si>
+    <t>N Tiến</t>
+  </si>
+  <si>
+    <t>X Tiến</t>
+  </si>
+  <si>
+    <t>Duy</t>
+  </si>
+  <si>
     <t>Vân</t>
   </si>
   <si>
-    <t>Ngọc Tiến</t>
-  </si>
-  <si>
-    <t>Công</t>
-  </si>
-  <si>
-    <t>Duy</t>
-  </si>
-  <si>
-    <t>X Tiến</t>
+    <t>21-22/10/2020</t>
+  </si>
+  <si>
+    <t>23-24/10/2020</t>
+  </si>
+  <si>
+    <t>23-26/10/2020</t>
+  </si>
+  <si>
+    <t>27-1/11/2020</t>
+  </si>
+  <si>
+    <t>03-07/11/2020</t>
+  </si>
+  <si>
+    <t>08-015/11/2020</t>
+  </si>
+  <si>
+    <t>16-17/11/2020</t>
   </si>
 </sst>
 </file>
@@ -150,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -160,11 +181,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -174,14 +190,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,7 +497,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,114 +517,130 @@
       <c r="D1" s="3"/>
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="36" x14ac:dyDescent="0.35">
-      <c r="A5" s="9">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="12" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
-        <v>4</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="9">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="9">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="10">
-        <v>8</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>